<commit_message>
add: reset password and search
</commit_message>
<xml_diff>
--- a/public/template/jurusan_template.xlsx
+++ b/public/template/jurusan_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Apang\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Apang\Documents\Template excel SIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFE4A1B-4194-4EE7-BAE9-F1774AA25687}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C717432-9DB6-496F-A41B-63B1F6B18DE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Kode Jurusan</t>
   </si>
@@ -33,44 +33,50 @@
     <t>Nama Jurusan</t>
   </si>
   <si>
-    <t>Akuakultur</t>
-  </si>
-  <si>
-    <t>Akuntansi</t>
-  </si>
-  <si>
-    <t>Hukum</t>
-  </si>
-  <si>
-    <t>Ilmu Hubungan Internasional</t>
-  </si>
-  <si>
-    <t>Ilmu Komunikasi</t>
-  </si>
-  <si>
-    <t>Magister Manajemen</t>
-  </si>
-  <si>
-    <t>Manajemen</t>
-  </si>
-  <si>
-    <t>Pemanfaatan Sumber Daya Perikanan</t>
-  </si>
-  <si>
-    <t>Sistem Informasi</t>
-  </si>
-  <si>
-    <t>Teknik Informatika</t>
-  </si>
-  <si>
-    <t>Teknik Lingkungan</t>
+    <t>S1 Akuakultur</t>
+  </si>
+  <si>
+    <t>S1 Akuntansi</t>
+  </si>
+  <si>
+    <t>S1 Hukum</t>
+  </si>
+  <si>
+    <t>S1 Ilmu Hubungan Internasional</t>
+  </si>
+  <si>
+    <t>S1 Ilmu Komunikasi</t>
+  </si>
+  <si>
+    <t>S2 Magister Manajemen</t>
+  </si>
+  <si>
+    <t>S1 Manajemen</t>
+  </si>
+  <si>
+    <t>S1 Pemanfaatan Sumber Daya Perikanan</t>
+  </si>
+  <si>
+    <t>S1 Sistem Informasi</t>
+  </si>
+  <si>
+    <t>S1 Teknik Informatika</t>
+  </si>
+  <si>
+    <t>S1 Teknik Lingkungan</t>
+  </si>
+  <si>
+    <t>57401</t>
+  </si>
+  <si>
+    <t>D3 Manajemen Informatika</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,11 +86,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -107,16 +118,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -398,16 +418,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -419,92 +440,100 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="6">
         <v>54250</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="6">
         <v>62201</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="6">
         <v>74201</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="6">
         <v>64201</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="6">
         <v>70201</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="6">
         <v>61101</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="6">
         <v>61201</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="6">
         <v>54246</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="6">
         <v>57201</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="6">
         <v>55201</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="6">
         <v>25201</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="6" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>